<commit_message>
uploading all reports, added data transformation (log transformation, normalization), removed unused files
</commit_message>
<xml_diff>
--- a/lfs_april_2016_metadata(dictionary).xlsx
+++ b/lfs_april_2016_metadata(dictionary).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cynicap\Documents\School\STINTSY\Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BDFD93C-B7BA-4ADC-8FB3-22D76B8B795B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD4F736C-1907-4ECC-B680-D088B09D070F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -3975,8 +3975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA194C70-7A58-425D-9E3E-461AE0A5F7F8}">
   <dimension ref="A1:V53"/>
   <sheetViews>
-    <sheetView topLeftCell="D21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="P28" sqref="P28"/>
+    <sheetView topLeftCell="C28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E53" sqref="E53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4682,8 +4682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F1144"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A162" zoomScale="96" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C183" sqref="C183"/>
+    <sheetView tabSelected="1" topLeftCell="A483" zoomScale="96" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H495" sqref="H495"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13836,5 +13836,6 @@
     <mergeCell ref="E137:E143"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>